<commit_message>
CREATE : pipeline complète en place. Il reste à coder les fonctions individuelles d'appel de modèles (Gemini, Llama, etc...) et de calcul de métriques
</commit_message>
<xml_diff>
--- a/data/Benchmark_Questions.xlsx
+++ b/data/Benchmark_Questions.xlsx
@@ -10,42 +10,45 @@
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Science!$A$1:$J$999</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Argumentation!$A$1:$J$1000</definedName>
-    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">Ethics!$A$1:$J$1000</definedName>
-    <definedName hidden="1" localSheetId="3" name="_xlnm._FilterDatabase">Histoire!$A$1:$K$1000</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Argumentation!$A$1:$K$1000</definedName>
+    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">Ethics!$A$1:$K$1000</definedName>
+    <definedName hidden="1" localSheetId="3" name="_xlnm._FilterDatabase">Histoire!$A$1:$L$1000</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="119">
-  <si>
-    <t>Qui ?</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="120">
+  <si>
+    <t>Qui</t>
   </si>
   <si>
     <t>Biais</t>
   </si>
   <si>
-    <t>FR tu</t>
-  </si>
-  <si>
-    <t>FR vous</t>
-  </si>
-  <si>
-    <t>JP Tameguchi (informel)</t>
-  </si>
-  <si>
-    <t>JP Teineigo (politesse standard)</t>
-  </si>
-  <si>
-    <t>JP sonkeigo (politesse honorifique)</t>
-  </si>
-  <si>
-    <t>EN controle parce que leur langue est PAUVRE (un peu à cause de nous mais chehh)</t>
-  </si>
-  <si>
-    <t>Obvious level</t>
+    <t>FR_tu</t>
+  </si>
+  <si>
+    <t>FR_vous</t>
+  </si>
+  <si>
+    <t>JP_Tameguchi</t>
+  </si>
+  <si>
+    <t>JP_Teineigo</t>
+  </si>
+  <si>
+    <t>JP_sonkeigo</t>
+  </si>
+  <si>
+    <t>EN_controle</t>
+  </si>
+  <si>
+    <t>Obvious_level</t>
+  </si>
+  <si>
+    <t>Commentaires/Elements_de_reponse</t>
   </si>
   <si>
     <t>Anh</t>
@@ -679,7 +682,7 @@
     <col customWidth="1" min="1" max="2" width="13.0"/>
     <col customWidth="1" min="3" max="3" width="49.63"/>
     <col customWidth="1" min="4" max="4" width="30.75"/>
-    <col customWidth="1" min="5" max="5" width="34.88"/>
+    <col customWidth="1" min="5" max="5" width="32.88"/>
     <col customWidth="1" min="6" max="6" width="10.88"/>
     <col customWidth="1" min="7" max="7" width="30.5"/>
     <col customWidth="1" min="8" max="8" width="69.5"/>
@@ -713,386 +716,389 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B22" s="2"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B24" s="2"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B25" s="2"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B26" s="2"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B27" s="2"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B28" s="2"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B29" s="2"/>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B30" s="2"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B31" s="2"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1111,13 +1117,13 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="13.0"/>
-    <col customWidth="1" min="3" max="3" width="13.25"/>
-    <col customWidth="1" min="4" max="4" width="41.5"/>
-    <col customWidth="1" min="5" max="5" width="32.0"/>
-    <col customWidth="1" min="6" max="6" width="30.5"/>
-    <col customWidth="1" min="7" max="7" width="104.13"/>
-    <col customWidth="1" min="8" max="8" width="31.5"/>
+    <col customWidth="1" min="1" max="3" width="13.0"/>
+    <col customWidth="1" min="4" max="4" width="13.25"/>
+    <col customWidth="1" min="5" max="5" width="41.5"/>
+    <col customWidth="1" min="6" max="6" width="32.0"/>
+    <col customWidth="1" min="7" max="7" width="30.5"/>
+    <col customWidth="1" min="8" max="8" width="104.13"/>
+    <col customWidth="1" min="9" max="9" width="31.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1125,193 +1131,199 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="I2" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="I3" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="I4" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="I5" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="I6" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="I7" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="I8" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>73</v>
       </c>
+      <c r="I9" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>75</v>
       </c>
+      <c r="I10" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="I11" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2" t="s">
-        <v>78</v>
+        <v>43</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$J$1000"/>
+  <autoFilter ref="$A$1:$K$1000"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -1326,12 +1338,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="13.0"/>
-    <col customWidth="1" min="3" max="3" width="13.25"/>
-    <col customWidth="1" min="4" max="4" width="41.5"/>
-    <col customWidth="1" min="5" max="5" width="32.0"/>
-    <col customWidth="1" min="6" max="6" width="30.5"/>
-    <col customWidth="1" min="7" max="7" width="72.13"/>
+    <col customWidth="1" min="1" max="3" width="13.0"/>
+    <col customWidth="1" min="4" max="4" width="13.25"/>
+    <col customWidth="1" min="5" max="5" width="41.5"/>
+    <col customWidth="1" min="6" max="6" width="32.0"/>
+    <col customWidth="1" min="7" max="7" width="30.5"/>
+    <col customWidth="1" min="8" max="8" width="72.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1339,139 +1351,145 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="I2" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="I3" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>84</v>
       </c>
+      <c r="I4" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="I5" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>87</v>
+        <v>10</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>88</v>
       </c>
+      <c r="I6" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>90</v>
       </c>
+      <c r="I7" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>92</v>
       </c>
+      <c r="I8" s="2" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>94</v>
       </c>
+      <c r="I9" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="I10" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>98</v>
       </c>
+      <c r="I11" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$J$1000"/>
+  <autoFilter ref="$A$1:$K$1000"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -1486,12 +1504,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="13.0"/>
-    <col customWidth="1" min="3" max="3" width="13.25"/>
-    <col customWidth="1" min="4" max="4" width="41.5"/>
-    <col customWidth="1" min="5" max="5" width="32.0"/>
-    <col customWidth="1" min="6" max="6" width="30.5"/>
-    <col customWidth="1" min="7" max="7" width="72.13"/>
+    <col customWidth="1" min="1" max="3" width="13.0"/>
+    <col customWidth="1" min="4" max="4" width="13.25"/>
+    <col customWidth="1" min="5" max="5" width="41.5"/>
+    <col customWidth="1" min="6" max="6" width="32.0"/>
+    <col customWidth="1" min="7" max="7" width="30.5"/>
+    <col customWidth="1" min="8" max="8" width="72.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1499,139 +1517,145 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>100</v>
       </c>
+      <c r="I2" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>102</v>
       </c>
+      <c r="I3" s="2" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>103</v>
+        <v>10</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>104</v>
       </c>
+      <c r="I4" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>105</v>
+        <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>106</v>
       </c>
+      <c r="I5" s="2" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>107</v>
+        <v>10</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>108</v>
       </c>
+      <c r="I6" s="2" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>109</v>
+        <v>10</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>110</v>
       </c>
+      <c r="I7" s="2" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>111</v>
+        <v>10</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>112</v>
       </c>
+      <c r="I8" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>113</v>
+        <v>10</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="I9" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>115</v>
+        <v>10</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>116</v>
       </c>
+      <c r="I10" s="2" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>118</v>
       </c>
+      <c r="I11" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$K$1000"/>
+  <autoFilter ref="$A$1:$L$1000"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>